<commit_message>
Removed aaa.py. Other changes shown in script.py
</commit_message>
<xml_diff>
--- a/orar.xlsx
+++ b/orar.xlsx
@@ -79,15 +79,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="5.0"/>
-      </rPr>
-      <t>SI-243</t>
-    </r>
+    <t>SI-243</t>
   </si>
   <si>
     <r>
@@ -761,15 +753,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="5.0"/>
-      </rPr>
-      <t>Marţi</t>
-    </r>
+    <t>Marţi</t>
   </si>
   <si>
     <r>
@@ -3997,7 +3981,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
@@ -4051,6 +4035,9 @@
     </xf>
     <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -4321,7 +4308,7 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -4604,7 +4591,7 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" ht="18.0" customHeight="1">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="18" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -4699,10 +4686,10 @@
       <c r="I20" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="J20" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K20" s="19"/>
+      <c r="K20" s="20"/>
       <c r="L20" s="2"/>
     </row>
     <row r="21" ht="18.0" customHeight="1">
@@ -4719,10 +4706,10 @@
       <c r="I21" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="J21" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="K21" s="19"/>
+      <c r="K21" s="20"/>
       <c r="L21" s="2"/>
     </row>
     <row r="22" ht="18.0" customHeight="1">
@@ -5338,13 +5325,13 @@
       <c r="B52" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="C52" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
       <c r="H52" s="2"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
@@ -5356,13 +5343,13 @@
     <row r="53" ht="18.0" customHeight="1">
       <c r="A53" s="8"/>
       <c r="B53" s="9"/>
-      <c r="C53" s="18" t="s">
+      <c r="C53" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
       <c r="H53" s="2"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
@@ -5471,22 +5458,22 @@
     </row>
     <row r="60" ht="18.0" customHeight="1">
       <c r="A60" s="8"/>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="C60" s="21"/>
+      <c r="C60" s="22"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
-      <c r="I60" s="20" t="s">
+      <c r="I60" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="J60" s="18" t="s">
+      <c r="J60" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="K60" s="19"/>
+      <c r="K60" s="20"/>
       <c r="L60" s="2"/>
     </row>
     <row r="61" ht="18.0" customHeight="1">
@@ -5496,42 +5483,42 @@
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
-      <c r="G61" s="22" t="s">
+      <c r="G61" s="23" t="s">
         <v>174</v>
       </c>
       <c r="H61" s="7"/>
       <c r="I61" s="9"/>
-      <c r="J61" s="23"/>
-      <c r="K61" s="22" t="s">
+      <c r="J61" s="24"/>
+      <c r="K61" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="L61" s="22" t="s">
+      <c r="L61" s="23" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="62" ht="18.0" customHeight="1">
       <c r="A62" s="8"/>
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="C62" s="21"/>
+      <c r="C62" s="22"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
-      <c r="G62" s="24" t="s">
+      <c r="G62" s="25" t="s">
         <v>178</v>
       </c>
       <c r="H62" s="7"/>
-      <c r="I62" s="25" t="s">
+      <c r="I62" s="26" t="s">
         <v>179</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="K62" s="20" t="s">
+      <c r="K62" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="L62" s="20" t="s">
+      <c r="L62" s="21" t="s">
         <v>182</v>
       </c>
     </row>
@@ -5573,7 +5560,7 @@
       <c r="K64" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="L64" s="20" t="s">
+      <c r="L64" s="21" t="s">
         <v>189</v>
       </c>
     </row>
@@ -5589,7 +5576,7 @@
       <c r="I65" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="J65" s="22" t="s">
+      <c r="J65" s="23" t="s">
         <v>191</v>
       </c>
       <c r="K65" s="9"/>
@@ -5619,11 +5606,11 @@
         <v>198</v>
       </c>
       <c r="I66" s="3"/>
-      <c r="J66" s="20" t="s">
+      <c r="J66" s="21" t="s">
         <v>199</v>
       </c>
       <c r="K66" s="7"/>
-      <c r="L66" s="20" t="s">
+      <c r="L66" s="21" t="s">
         <v>200</v>
       </c>
     </row>
@@ -5690,13 +5677,13 @@
       <c r="B70" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C70" s="18" t="s">
+      <c r="C70" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="D70" s="19"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="19"/>
-      <c r="G70" s="19"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
       <c r="H70" s="2"/>
       <c r="I70" s="7"/>
       <c r="J70" s="6"/>
@@ -5722,808 +5709,808 @@
       <c r="L71" s="9"/>
     </row>
     <row r="72" ht="18.0" customHeight="1">
-      <c r="A72" s="26"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27"/>
-      <c r="I72" s="27"/>
-      <c r="J72" s="27"/>
-      <c r="K72" s="27"/>
-      <c r="L72" s="27"/>
+      <c r="A72" s="27"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="28"/>
+      <c r="G72" s="28"/>
+      <c r="H72" s="28"/>
+      <c r="I72" s="28"/>
+      <c r="J72" s="28"/>
+      <c r="K72" s="28"/>
+      <c r="L72" s="28"/>
     </row>
     <row r="73" ht="18.0" customHeight="1">
-      <c r="A73" s="26"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="27"/>
-      <c r="H73" s="27"/>
-      <c r="I73" s="27"/>
-      <c r="J73" s="27"/>
-      <c r="K73" s="27"/>
-      <c r="L73" s="27"/>
+      <c r="A73" s="27"/>
+      <c r="B73" s="27"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
+      <c r="G73" s="28"/>
+      <c r="H73" s="28"/>
+      <c r="I73" s="28"/>
+      <c r="J73" s="28"/>
+      <c r="K73" s="28"/>
+      <c r="L73" s="28"/>
     </row>
     <row r="74" ht="18.0" customHeight="1">
-      <c r="A74" s="26"/>
-      <c r="B74" s="26"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="27"/>
-      <c r="F74" s="27"/>
-      <c r="G74" s="27"/>
-      <c r="H74" s="27"/>
-      <c r="I74" s="27"/>
-      <c r="J74" s="27"/>
-      <c r="K74" s="27"/>
-      <c r="L74" s="27"/>
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="28"/>
+      <c r="G74" s="28"/>
+      <c r="H74" s="28"/>
+      <c r="I74" s="28"/>
+      <c r="J74" s="28"/>
+      <c r="K74" s="28"/>
+      <c r="L74" s="28"/>
     </row>
     <row r="75" ht="18.0" customHeight="1">
-      <c r="A75" s="26"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="27"/>
-      <c r="H75" s="27"/>
-      <c r="I75" s="27"/>
-      <c r="J75" s="27"/>
-      <c r="K75" s="27"/>
-      <c r="L75" s="27"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="28"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="28"/>
+      <c r="I75" s="28"/>
+      <c r="J75" s="28"/>
+      <c r="K75" s="28"/>
+      <c r="L75" s="28"/>
     </row>
     <row r="76" ht="18.0" customHeight="1">
-      <c r="A76" s="26"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="27"/>
-      <c r="H76" s="27"/>
-      <c r="I76" s="27"/>
-      <c r="J76" s="27"/>
-      <c r="K76" s="27"/>
-      <c r="L76" s="27"/>
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="28"/>
+      <c r="F76" s="28"/>
+      <c r="G76" s="28"/>
+      <c r="H76" s="28"/>
+      <c r="I76" s="28"/>
+      <c r="J76" s="28"/>
+      <c r="K76" s="28"/>
+      <c r="L76" s="28"/>
     </row>
     <row r="77" ht="18.0" customHeight="1">
-      <c r="A77" s="26"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="27"/>
-      <c r="H77" s="27"/>
-      <c r="I77" s="27"/>
-      <c r="J77" s="27"/>
-      <c r="K77" s="27"/>
-      <c r="L77" s="27"/>
+      <c r="A77" s="27"/>
+      <c r="B77" s="27"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="28"/>
+      <c r="F77" s="28"/>
+      <c r="G77" s="28"/>
+      <c r="H77" s="28"/>
+      <c r="I77" s="28"/>
+      <c r="J77" s="28"/>
+      <c r="K77" s="28"/>
+      <c r="L77" s="28"/>
     </row>
     <row r="78" ht="18.0" customHeight="1">
-      <c r="A78" s="26"/>
-      <c r="B78" s="26"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
-      <c r="F78" s="27"/>
-      <c r="G78" s="27"/>
-      <c r="H78" s="27"/>
-      <c r="I78" s="27"/>
-      <c r="J78" s="27"/>
-      <c r="K78" s="27"/>
-      <c r="L78" s="27"/>
+      <c r="A78" s="27"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="28"/>
+      <c r="F78" s="28"/>
+      <c r="G78" s="28"/>
+      <c r="H78" s="28"/>
+      <c r="I78" s="28"/>
+      <c r="J78" s="28"/>
+      <c r="K78" s="28"/>
+      <c r="L78" s="28"/>
     </row>
     <row r="79" ht="18.0" customHeight="1">
-      <c r="A79" s="26"/>
-      <c r="B79" s="26"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
-      <c r="E79" s="27"/>
-      <c r="F79" s="27"/>
-      <c r="G79" s="27"/>
-      <c r="H79" s="27"/>
-      <c r="I79" s="27"/>
-      <c r="J79" s="27"/>
-      <c r="K79" s="27"/>
-      <c r="L79" s="27"/>
+      <c r="A79" s="27"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="28"/>
+      <c r="F79" s="28"/>
+      <c r="G79" s="28"/>
+      <c r="H79" s="28"/>
+      <c r="I79" s="28"/>
+      <c r="J79" s="28"/>
+      <c r="K79" s="28"/>
+      <c r="L79" s="28"/>
     </row>
     <row r="80" ht="18.0" customHeight="1">
-      <c r="A80" s="26"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27"/>
-      <c r="H80" s="27"/>
-      <c r="I80" s="27"/>
-      <c r="J80" s="27"/>
-      <c r="K80" s="27"/>
-      <c r="L80" s="27"/>
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="28"/>
+      <c r="G80" s="28"/>
+      <c r="H80" s="28"/>
+      <c r="I80" s="28"/>
+      <c r="J80" s="28"/>
+      <c r="K80" s="28"/>
+      <c r="L80" s="28"/>
     </row>
     <row r="81" ht="18.0" customHeight="1">
-      <c r="A81" s="26"/>
-      <c r="B81" s="26"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="27"/>
-      <c r="H81" s="27"/>
-      <c r="I81" s="27"/>
-      <c r="J81" s="27"/>
-      <c r="K81" s="27"/>
-      <c r="L81" s="27"/>
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="28"/>
+      <c r="F81" s="28"/>
+      <c r="G81" s="28"/>
+      <c r="H81" s="28"/>
+      <c r="I81" s="28"/>
+      <c r="J81" s="28"/>
+      <c r="K81" s="28"/>
+      <c r="L81" s="28"/>
     </row>
     <row r="82" ht="18.0" customHeight="1">
-      <c r="A82" s="26"/>
-      <c r="B82" s="26"/>
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27"/>
-      <c r="F82" s="27"/>
-      <c r="G82" s="27"/>
-      <c r="H82" s="27"/>
-      <c r="I82" s="27"/>
-      <c r="J82" s="27"/>
-      <c r="K82" s="27"/>
-      <c r="L82" s="27"/>
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="28"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="28"/>
+      <c r="F82" s="28"/>
+      <c r="G82" s="28"/>
+      <c r="H82" s="28"/>
+      <c r="I82" s="28"/>
+      <c r="J82" s="28"/>
+      <c r="K82" s="28"/>
+      <c r="L82" s="28"/>
     </row>
     <row r="83" ht="18.0" customHeight="1">
-      <c r="A83" s="26"/>
-      <c r="B83" s="26"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="27"/>
-      <c r="H83" s="27"/>
-      <c r="I83" s="27"/>
-      <c r="J83" s="27"/>
-      <c r="K83" s="27"/>
-      <c r="L83" s="27"/>
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="28"/>
+      <c r="G83" s="28"/>
+      <c r="H83" s="28"/>
+      <c r="I83" s="28"/>
+      <c r="J83" s="28"/>
+      <c r="K83" s="28"/>
+      <c r="L83" s="28"/>
     </row>
     <row r="84" ht="18.0" customHeight="1">
-      <c r="A84" s="26"/>
-      <c r="B84" s="26"/>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="27"/>
-      <c r="H84" s="27"/>
-      <c r="I84" s="27"/>
-      <c r="J84" s="27"/>
-      <c r="K84" s="27"/>
-      <c r="L84" s="27"/>
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="28"/>
+      <c r="F84" s="28"/>
+      <c r="G84" s="28"/>
+      <c r="H84" s="28"/>
+      <c r="I84" s="28"/>
+      <c r="J84" s="28"/>
+      <c r="K84" s="28"/>
+      <c r="L84" s="28"/>
     </row>
     <row r="85" ht="18.0" customHeight="1">
-      <c r="A85" s="26"/>
-      <c r="B85" s="26"/>
-      <c r="C85" s="27"/>
-      <c r="D85" s="27"/>
-      <c r="E85" s="27"/>
-      <c r="F85" s="27"/>
-      <c r="G85" s="27"/>
-      <c r="H85" s="27"/>
-      <c r="I85" s="27"/>
-      <c r="J85" s="27"/>
-      <c r="K85" s="27"/>
-      <c r="L85" s="27"/>
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="28"/>
+      <c r="F85" s="28"/>
+      <c r="G85" s="28"/>
+      <c r="H85" s="28"/>
+      <c r="I85" s="28"/>
+      <c r="J85" s="28"/>
+      <c r="K85" s="28"/>
+      <c r="L85" s="28"/>
     </row>
     <row r="86" ht="18.0" customHeight="1">
-      <c r="A86" s="26"/>
-      <c r="B86" s="26"/>
-      <c r="C86" s="27"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="27"/>
-      <c r="F86" s="27"/>
-      <c r="G86" s="27"/>
-      <c r="H86" s="27"/>
-      <c r="I86" s="27"/>
-      <c r="J86" s="27"/>
-      <c r="K86" s="27"/>
-      <c r="L86" s="27"/>
+      <c r="A86" s="27"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="28"/>
+      <c r="F86" s="28"/>
+      <c r="G86" s="28"/>
+      <c r="H86" s="28"/>
+      <c r="I86" s="28"/>
+      <c r="J86" s="28"/>
+      <c r="K86" s="28"/>
+      <c r="L86" s="28"/>
     </row>
     <row r="87" ht="18.0" customHeight="1">
-      <c r="A87" s="26"/>
-      <c r="B87" s="26"/>
-      <c r="C87" s="27"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
-      <c r="G87" s="27"/>
-      <c r="H87" s="27"/>
-      <c r="I87" s="27"/>
-      <c r="J87" s="27"/>
-      <c r="K87" s="27"/>
-      <c r="L87" s="27"/>
+      <c r="A87" s="27"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="28"/>
+      <c r="E87" s="28"/>
+      <c r="F87" s="28"/>
+      <c r="G87" s="28"/>
+      <c r="H87" s="28"/>
+      <c r="I87" s="28"/>
+      <c r="J87" s="28"/>
+      <c r="K87" s="28"/>
+      <c r="L87" s="28"/>
     </row>
     <row r="88" ht="18.0" customHeight="1">
-      <c r="A88" s="26"/>
-      <c r="B88" s="26"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
-      <c r="G88" s="27"/>
-      <c r="H88" s="27"/>
-      <c r="I88" s="27"/>
-      <c r="J88" s="27"/>
-      <c r="K88" s="27"/>
-      <c r="L88" s="27"/>
+      <c r="A88" s="27"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="28"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="28"/>
+      <c r="H88" s="28"/>
+      <c r="I88" s="28"/>
+      <c r="J88" s="28"/>
+      <c r="K88" s="28"/>
+      <c r="L88" s="28"/>
     </row>
     <row r="89" ht="18.0" customHeight="1">
-      <c r="A89" s="26"/>
-      <c r="B89" s="26"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
-      <c r="J89" s="27"/>
-      <c r="K89" s="27"/>
-      <c r="L89" s="27"/>
+      <c r="A89" s="27"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="28"/>
+      <c r="G89" s="28"/>
+      <c r="H89" s="28"/>
+      <c r="I89" s="28"/>
+      <c r="J89" s="28"/>
+      <c r="K89" s="28"/>
+      <c r="L89" s="28"/>
     </row>
     <row r="90" ht="18.0" customHeight="1">
-      <c r="A90" s="26"/>
-      <c r="B90" s="26"/>
-      <c r="C90" s="27"/>
-      <c r="D90" s="27"/>
-      <c r="E90" s="27"/>
-      <c r="F90" s="27"/>
-      <c r="G90" s="27"/>
-      <c r="H90" s="27"/>
-      <c r="I90" s="27"/>
-      <c r="J90" s="27"/>
-      <c r="K90" s="27"/>
-      <c r="L90" s="27"/>
+      <c r="A90" s="27"/>
+      <c r="B90" s="27"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="28"/>
+      <c r="G90" s="28"/>
+      <c r="H90" s="28"/>
+      <c r="I90" s="28"/>
+      <c r="J90" s="28"/>
+      <c r="K90" s="28"/>
+      <c r="L90" s="28"/>
     </row>
     <row r="91" ht="18.0" customHeight="1">
-      <c r="A91" s="26"/>
-      <c r="B91" s="26"/>
-      <c r="C91" s="27"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="27"/>
-      <c r="F91" s="27"/>
-      <c r="G91" s="27"/>
-      <c r="H91" s="27"/>
-      <c r="I91" s="27"/>
-      <c r="J91" s="27"/>
-      <c r="K91" s="27"/>
-      <c r="L91" s="27"/>
+      <c r="A91" s="27"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="28"/>
+      <c r="G91" s="28"/>
+      <c r="H91" s="28"/>
+      <c r="I91" s="28"/>
+      <c r="J91" s="28"/>
+      <c r="K91" s="28"/>
+      <c r="L91" s="28"/>
     </row>
     <row r="92" ht="18.0" customHeight="1">
-      <c r="A92" s="26"/>
-      <c r="B92" s="26"/>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
-      <c r="G92" s="27"/>
-      <c r="H92" s="27"/>
-      <c r="I92" s="27"/>
-      <c r="J92" s="27"/>
-      <c r="K92" s="27"/>
-      <c r="L92" s="27"/>
+      <c r="A92" s="27"/>
+      <c r="B92" s="27"/>
+      <c r="C92" s="28"/>
+      <c r="D92" s="28"/>
+      <c r="E92" s="28"/>
+      <c r="F92" s="28"/>
+      <c r="G92" s="28"/>
+      <c r="H92" s="28"/>
+      <c r="I92" s="28"/>
+      <c r="J92" s="28"/>
+      <c r="K92" s="28"/>
+      <c r="L92" s="28"/>
     </row>
     <row r="93" ht="18.0" customHeight="1">
-      <c r="A93" s="26"/>
-      <c r="B93" s="26"/>
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
-      <c r="G93" s="27"/>
-      <c r="H93" s="27"/>
-      <c r="I93" s="27"/>
-      <c r="J93" s="27"/>
-      <c r="K93" s="27"/>
-      <c r="L93" s="27"/>
+      <c r="A93" s="27"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="28"/>
+      <c r="E93" s="28"/>
+      <c r="F93" s="28"/>
+      <c r="G93" s="28"/>
+      <c r="H93" s="28"/>
+      <c r="I93" s="28"/>
+      <c r="J93" s="28"/>
+      <c r="K93" s="28"/>
+      <c r="L93" s="28"/>
     </row>
     <row r="94" ht="18.0" customHeight="1">
-      <c r="A94" s="26"/>
-      <c r="B94" s="26"/>
-      <c r="C94" s="27"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="27"/>
-      <c r="F94" s="27"/>
-      <c r="G94" s="27"/>
-      <c r="H94" s="27"/>
-      <c r="I94" s="27"/>
-      <c r="J94" s="27"/>
-      <c r="K94" s="27"/>
-      <c r="L94" s="27"/>
+      <c r="A94" s="27"/>
+      <c r="B94" s="27"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="28"/>
+      <c r="E94" s="28"/>
+      <c r="F94" s="28"/>
+      <c r="G94" s="28"/>
+      <c r="H94" s="28"/>
+      <c r="I94" s="28"/>
+      <c r="J94" s="28"/>
+      <c r="K94" s="28"/>
+      <c r="L94" s="28"/>
     </row>
     <row r="95" ht="18.0" customHeight="1">
-      <c r="A95" s="26"/>
-      <c r="B95" s="26"/>
-      <c r="C95" s="27"/>
-      <c r="D95" s="27"/>
-      <c r="E95" s="27"/>
-      <c r="F95" s="27"/>
-      <c r="G95" s="27"/>
-      <c r="H95" s="27"/>
-      <c r="I95" s="27"/>
-      <c r="J95" s="27"/>
-      <c r="K95" s="27"/>
-      <c r="L95" s="27"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="28"/>
+      <c r="E95" s="28"/>
+      <c r="F95" s="28"/>
+      <c r="G95" s="28"/>
+      <c r="H95" s="28"/>
+      <c r="I95" s="28"/>
+      <c r="J95" s="28"/>
+      <c r="K95" s="28"/>
+      <c r="L95" s="28"/>
     </row>
     <row r="96" ht="18.0" customHeight="1">
-      <c r="A96" s="26"/>
-      <c r="B96" s="26"/>
-      <c r="C96" s="27"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="27"/>
-      <c r="F96" s="27"/>
-      <c r="G96" s="27"/>
-      <c r="H96" s="27"/>
-      <c r="I96" s="27"/>
-      <c r="J96" s="27"/>
-      <c r="K96" s="27"/>
-      <c r="L96" s="27"/>
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="28"/>
+      <c r="F96" s="28"/>
+      <c r="G96" s="28"/>
+      <c r="H96" s="28"/>
+      <c r="I96" s="28"/>
+      <c r="J96" s="28"/>
+      <c r="K96" s="28"/>
+      <c r="L96" s="28"/>
     </row>
     <row r="97" ht="18.0" customHeight="1">
-      <c r="A97" s="26"/>
-      <c r="B97" s="26"/>
-      <c r="C97" s="27"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="27"/>
-      <c r="H97" s="27"/>
-      <c r="I97" s="27"/>
-      <c r="J97" s="27"/>
-      <c r="K97" s="27"/>
-      <c r="L97" s="27"/>
+      <c r="A97" s="27"/>
+      <c r="B97" s="27"/>
+      <c r="C97" s="28"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="28"/>
+      <c r="F97" s="28"/>
+      <c r="G97" s="28"/>
+      <c r="H97" s="28"/>
+      <c r="I97" s="28"/>
+      <c r="J97" s="28"/>
+      <c r="K97" s="28"/>
+      <c r="L97" s="28"/>
     </row>
     <row r="98" ht="18.0" customHeight="1">
-      <c r="A98" s="26"/>
-      <c r="B98" s="26"/>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
-      <c r="H98" s="27"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="27"/>
-      <c r="K98" s="27"/>
-      <c r="L98" s="27"/>
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="28"/>
+      <c r="H98" s="28"/>
+      <c r="I98" s="28"/>
+      <c r="J98" s="28"/>
+      <c r="K98" s="28"/>
+      <c r="L98" s="28"/>
     </row>
     <row r="99" ht="18.0" customHeight="1">
-      <c r="A99" s="26"/>
-      <c r="B99" s="26"/>
-      <c r="C99" s="27"/>
-      <c r="D99" s="27"/>
-      <c r="E99" s="27"/>
-      <c r="F99" s="27"/>
-      <c r="G99" s="27"/>
-      <c r="H99" s="27"/>
-      <c r="I99" s="27"/>
-      <c r="J99" s="27"/>
-      <c r="K99" s="27"/>
-      <c r="L99" s="27"/>
+      <c r="A99" s="27"/>
+      <c r="B99" s="27"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="28"/>
+      <c r="F99" s="28"/>
+      <c r="G99" s="28"/>
+      <c r="H99" s="28"/>
+      <c r="I99" s="28"/>
+      <c r="J99" s="28"/>
+      <c r="K99" s="28"/>
+      <c r="L99" s="28"/>
     </row>
     <row r="100" ht="18.0" customHeight="1">
-      <c r="A100" s="26"/>
-      <c r="B100" s="26"/>
-      <c r="C100" s="27"/>
-      <c r="D100" s="27"/>
-      <c r="E100" s="27"/>
-      <c r="F100" s="27"/>
-      <c r="G100" s="27"/>
-      <c r="H100" s="27"/>
-      <c r="I100" s="27"/>
-      <c r="J100" s="27"/>
-      <c r="K100" s="27"/>
-      <c r="L100" s="27"/>
+      <c r="A100" s="27"/>
+      <c r="B100" s="27"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="28"/>
+      <c r="E100" s="28"/>
+      <c r="F100" s="28"/>
+      <c r="G100" s="28"/>
+      <c r="H100" s="28"/>
+      <c r="I100" s="28"/>
+      <c r="J100" s="28"/>
+      <c r="K100" s="28"/>
+      <c r="L100" s="28"/>
     </row>
     <row r="101" ht="18.0" customHeight="1">
-      <c r="A101" s="26"/>
-      <c r="B101" s="26"/>
-      <c r="C101" s="27"/>
-      <c r="D101" s="27"/>
-      <c r="E101" s="27"/>
-      <c r="F101" s="27"/>
-      <c r="G101" s="27"/>
-      <c r="H101" s="27"/>
-      <c r="I101" s="27"/>
-      <c r="J101" s="27"/>
-      <c r="K101" s="27"/>
-      <c r="L101" s="27"/>
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="28"/>
+      <c r="E101" s="28"/>
+      <c r="F101" s="28"/>
+      <c r="G101" s="28"/>
+      <c r="H101" s="28"/>
+      <c r="I101" s="28"/>
+      <c r="J101" s="28"/>
+      <c r="K101" s="28"/>
+      <c r="L101" s="28"/>
     </row>
     <row r="102" ht="18.0" customHeight="1">
-      <c r="A102" s="26"/>
-      <c r="B102" s="26"/>
-      <c r="C102" s="27"/>
-      <c r="D102" s="27"/>
-      <c r="E102" s="27"/>
-      <c r="F102" s="27"/>
-      <c r="G102" s="27"/>
-      <c r="H102" s="27"/>
-      <c r="I102" s="27"/>
-      <c r="J102" s="27"/>
-      <c r="K102" s="27"/>
-      <c r="L102" s="27"/>
+      <c r="A102" s="27"/>
+      <c r="B102" s="27"/>
+      <c r="C102" s="28"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="28"/>
+      <c r="F102" s="28"/>
+      <c r="G102" s="28"/>
+      <c r="H102" s="28"/>
+      <c r="I102" s="28"/>
+      <c r="J102" s="28"/>
+      <c r="K102" s="28"/>
+      <c r="L102" s="28"/>
     </row>
     <row r="103" ht="18.0" customHeight="1">
-      <c r="A103" s="26"/>
-      <c r="B103" s="26"/>
-      <c r="C103" s="27"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="27"/>
-      <c r="F103" s="27"/>
-      <c r="G103" s="27"/>
-      <c r="H103" s="27"/>
-      <c r="I103" s="27"/>
-      <c r="J103" s="27"/>
-      <c r="K103" s="27"/>
-      <c r="L103" s="27"/>
+      <c r="A103" s="27"/>
+      <c r="B103" s="27"/>
+      <c r="C103" s="28"/>
+      <c r="D103" s="28"/>
+      <c r="E103" s="28"/>
+      <c r="F103" s="28"/>
+      <c r="G103" s="28"/>
+      <c r="H103" s="28"/>
+      <c r="I103" s="28"/>
+      <c r="J103" s="28"/>
+      <c r="K103" s="28"/>
+      <c r="L103" s="28"/>
     </row>
     <row r="104" ht="18.0" customHeight="1">
-      <c r="A104" s="26"/>
-      <c r="B104" s="26"/>
-      <c r="C104" s="27"/>
-      <c r="D104" s="27"/>
-      <c r="E104" s="27"/>
-      <c r="F104" s="27"/>
-      <c r="G104" s="27"/>
-      <c r="H104" s="27"/>
-      <c r="I104" s="27"/>
-      <c r="J104" s="27"/>
-      <c r="K104" s="27"/>
-      <c r="L104" s="27"/>
+      <c r="A104" s="27"/>
+      <c r="B104" s="27"/>
+      <c r="C104" s="28"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="28"/>
+      <c r="F104" s="28"/>
+      <c r="G104" s="28"/>
+      <c r="H104" s="28"/>
+      <c r="I104" s="28"/>
+      <c r="J104" s="28"/>
+      <c r="K104" s="28"/>
+      <c r="L104" s="28"/>
     </row>
     <row r="105" ht="18.0" customHeight="1">
-      <c r="A105" s="26"/>
-      <c r="B105" s="26"/>
-      <c r="C105" s="27"/>
-      <c r="D105" s="27"/>
-      <c r="E105" s="27"/>
-      <c r="F105" s="27"/>
-      <c r="G105" s="27"/>
-      <c r="H105" s="27"/>
-      <c r="I105" s="27"/>
-      <c r="J105" s="27"/>
-      <c r="K105" s="27"/>
-      <c r="L105" s="27"/>
+      <c r="A105" s="27"/>
+      <c r="B105" s="27"/>
+      <c r="C105" s="28"/>
+      <c r="D105" s="28"/>
+      <c r="E105" s="28"/>
+      <c r="F105" s="28"/>
+      <c r="G105" s="28"/>
+      <c r="H105" s="28"/>
+      <c r="I105" s="28"/>
+      <c r="J105" s="28"/>
+      <c r="K105" s="28"/>
+      <c r="L105" s="28"/>
     </row>
     <row r="106" ht="18.0" customHeight="1">
-      <c r="A106" s="26"/>
-      <c r="B106" s="26"/>
-      <c r="C106" s="27"/>
-      <c r="D106" s="27"/>
-      <c r="E106" s="27"/>
-      <c r="F106" s="27"/>
-      <c r="G106" s="27"/>
-      <c r="H106" s="27"/>
-      <c r="I106" s="27"/>
-      <c r="J106" s="27"/>
-      <c r="K106" s="27"/>
-      <c r="L106" s="27"/>
+      <c r="A106" s="27"/>
+      <c r="B106" s="27"/>
+      <c r="C106" s="28"/>
+      <c r="D106" s="28"/>
+      <c r="E106" s="28"/>
+      <c r="F106" s="28"/>
+      <c r="G106" s="28"/>
+      <c r="H106" s="28"/>
+      <c r="I106" s="28"/>
+      <c r="J106" s="28"/>
+      <c r="K106" s="28"/>
+      <c r="L106" s="28"/>
     </row>
     <row r="107" ht="18.0" customHeight="1">
-      <c r="A107" s="26"/>
-      <c r="B107" s="26"/>
-      <c r="C107" s="27"/>
-      <c r="D107" s="27"/>
-      <c r="E107" s="27"/>
-      <c r="F107" s="27"/>
-      <c r="G107" s="27"/>
-      <c r="H107" s="27"/>
-      <c r="I107" s="27"/>
-      <c r="J107" s="27"/>
-      <c r="K107" s="27"/>
-      <c r="L107" s="27"/>
+      <c r="A107" s="27"/>
+      <c r="B107" s="27"/>
+      <c r="C107" s="28"/>
+      <c r="D107" s="28"/>
+      <c r="E107" s="28"/>
+      <c r="F107" s="28"/>
+      <c r="G107" s="28"/>
+      <c r="H107" s="28"/>
+      <c r="I107" s="28"/>
+      <c r="J107" s="28"/>
+      <c r="K107" s="28"/>
+      <c r="L107" s="28"/>
     </row>
     <row r="108" ht="18.0" customHeight="1">
-      <c r="A108" s="26"/>
-      <c r="B108" s="26"/>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-      <c r="F108" s="27"/>
-      <c r="G108" s="27"/>
-      <c r="H108" s="27"/>
-      <c r="I108" s="27"/>
-      <c r="J108" s="27"/>
-      <c r="K108" s="27"/>
-      <c r="L108" s="27"/>
+      <c r="A108" s="27"/>
+      <c r="B108" s="27"/>
+      <c r="C108" s="28"/>
+      <c r="D108" s="28"/>
+      <c r="E108" s="28"/>
+      <c r="F108" s="28"/>
+      <c r="G108" s="28"/>
+      <c r="H108" s="28"/>
+      <c r="I108" s="28"/>
+      <c r="J108" s="28"/>
+      <c r="K108" s="28"/>
+      <c r="L108" s="28"/>
     </row>
     <row r="109" ht="18.0" customHeight="1">
-      <c r="A109" s="26"/>
-      <c r="B109" s="26"/>
-      <c r="C109" s="27"/>
-      <c r="D109" s="27"/>
-      <c r="E109" s="27"/>
-      <c r="F109" s="27"/>
-      <c r="G109" s="27"/>
-      <c r="H109" s="27"/>
-      <c r="I109" s="27"/>
-      <c r="J109" s="27"/>
-      <c r="K109" s="27"/>
-      <c r="L109" s="27"/>
+      <c r="A109" s="27"/>
+      <c r="B109" s="27"/>
+      <c r="C109" s="28"/>
+      <c r="D109" s="28"/>
+      <c r="E109" s="28"/>
+      <c r="F109" s="28"/>
+      <c r="G109" s="28"/>
+      <c r="H109" s="28"/>
+      <c r="I109" s="28"/>
+      <c r="J109" s="28"/>
+      <c r="K109" s="28"/>
+      <c r="L109" s="28"/>
     </row>
     <row r="110" ht="18.0" customHeight="1">
-      <c r="A110" s="26"/>
-      <c r="B110" s="26"/>
-      <c r="C110" s="27"/>
-      <c r="D110" s="27"/>
-      <c r="E110" s="27"/>
-      <c r="F110" s="27"/>
-      <c r="G110" s="27"/>
-      <c r="H110" s="27"/>
-      <c r="I110" s="27"/>
-      <c r="J110" s="27"/>
-      <c r="K110" s="27"/>
-      <c r="L110" s="27"/>
+      <c r="A110" s="27"/>
+      <c r="B110" s="27"/>
+      <c r="C110" s="28"/>
+      <c r="D110" s="28"/>
+      <c r="E110" s="28"/>
+      <c r="F110" s="28"/>
+      <c r="G110" s="28"/>
+      <c r="H110" s="28"/>
+      <c r="I110" s="28"/>
+      <c r="J110" s="28"/>
+      <c r="K110" s="28"/>
+      <c r="L110" s="28"/>
     </row>
     <row r="111" ht="18.0" customHeight="1">
-      <c r="A111" s="26"/>
-      <c r="B111" s="26"/>
-      <c r="C111" s="27"/>
-      <c r="D111" s="27"/>
-      <c r="E111" s="27"/>
-      <c r="F111" s="27"/>
-      <c r="G111" s="27"/>
-      <c r="H111" s="27"/>
-      <c r="I111" s="27"/>
-      <c r="J111" s="27"/>
-      <c r="K111" s="27"/>
-      <c r="L111" s="27"/>
+      <c r="A111" s="27"/>
+      <c r="B111" s="27"/>
+      <c r="C111" s="28"/>
+      <c r="D111" s="28"/>
+      <c r="E111" s="28"/>
+      <c r="F111" s="28"/>
+      <c r="G111" s="28"/>
+      <c r="H111" s="28"/>
+      <c r="I111" s="28"/>
+      <c r="J111" s="28"/>
+      <c r="K111" s="28"/>
+      <c r="L111" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="241">
-    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="A30:A43"/>
+    <mergeCell ref="A44:A57"/>
+    <mergeCell ref="A58:A71"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A16:A29"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B48:B49"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="C2:C3"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:H5"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="K4:K5"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:H7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:L7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
+    <mergeCell ref="J8:L9"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:G3"/>
     <mergeCell ref="F8:F11"/>
-    <mergeCell ref="H8:H9"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:L9"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="A2:A15"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A16:A29"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="J16:L17"/>
-    <mergeCell ref="J18:L19"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="J36:L37"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="J68:J69"/>
-    <mergeCell ref="K68:K69"/>
-    <mergeCell ref="I68:I69"/>
-    <mergeCell ref="K62:K63"/>
-    <mergeCell ref="L62:L63"/>
-    <mergeCell ref="J62:J63"/>
-    <mergeCell ref="J66:J67"/>
-    <mergeCell ref="K64:K65"/>
-    <mergeCell ref="L64:L65"/>
-    <mergeCell ref="L66:L69"/>
-    <mergeCell ref="I62:I63"/>
-    <mergeCell ref="C53:H53"/>
-    <mergeCell ref="J60:L60"/>
-    <mergeCell ref="C54:H55"/>
-    <mergeCell ref="C56:H57"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="K58:K59"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="J50:J51"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="J52:J53"/>
-    <mergeCell ref="K52:K53"/>
-    <mergeCell ref="L52:L53"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="K50:K51"/>
-    <mergeCell ref="L50:L51"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="H68:H69"/>
-    <mergeCell ref="C64:H65"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="H66:H67"/>
-    <mergeCell ref="J40:J41"/>
-    <mergeCell ref="K40:K42"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="C42:H43"/>
-    <mergeCell ref="C18:C19"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:L19"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="G20:G21"/>
     <mergeCell ref="H20:H21"/>
     <mergeCell ref="J20:L20"/>
     <mergeCell ref="J21:L21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="K34:K35"/>
     <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A30:A43"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J38:L39"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="J36:L37"/>
     <mergeCell ref="E38:E39"/>
     <mergeCell ref="F38:F39"/>
     <mergeCell ref="G38:G39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="J38:L39"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="K44:K45"/>
+    <mergeCell ref="L70:L71"/>
+    <mergeCell ref="L62:L63"/>
+    <mergeCell ref="L64:L65"/>
+    <mergeCell ref="L66:L69"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="K52:K53"/>
+    <mergeCell ref="K58:K59"/>
+    <mergeCell ref="J60:L60"/>
+    <mergeCell ref="K62:K63"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="J66:J67"/>
+    <mergeCell ref="K64:K65"/>
+    <mergeCell ref="I62:I63"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="I68:I69"/>
+    <mergeCell ref="J68:J69"/>
+    <mergeCell ref="K68:K69"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="K70:K71"/>
+    <mergeCell ref="H68:H69"/>
+    <mergeCell ref="C70:H70"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="C64:H65"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="H66:H67"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="K40:K42"/>
     <mergeCell ref="L40:L41"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="C42:H43"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
     <mergeCell ref="G46:G47"/>
     <mergeCell ref="H46:H47"/>
     <mergeCell ref="I46:I47"/>
     <mergeCell ref="J46:J47"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="I44:I45"/>
-    <mergeCell ref="J44:J45"/>
-    <mergeCell ref="K44:K45"/>
     <mergeCell ref="L46:L47"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="K48:K49"/>
-    <mergeCell ref="L48:L49"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
     <mergeCell ref="E48:E49"/>
     <mergeCell ref="F48:F49"/>
     <mergeCell ref="G48:G49"/>
     <mergeCell ref="H48:H49"/>
     <mergeCell ref="I48:I49"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A44:A57"/>
-    <mergeCell ref="A58:A71"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C70:H70"/>
-    <mergeCell ref="J70:J71"/>
-    <mergeCell ref="K70:K71"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="L70:L71"/>
+    <mergeCell ref="K48:K49"/>
+    <mergeCell ref="L48:L49"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="K50:K51"/>
+    <mergeCell ref="L50:L51"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="L52:L53"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="C53:H53"/>
+    <mergeCell ref="C54:H55"/>
+    <mergeCell ref="C56:H57"/>
+    <mergeCell ref="I58:I59"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="J16:L17"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>